<commit_message>
original link for scrapping has been added
</commit_message>
<xml_diff>
--- a/web-scraping/job.xlsx
+++ b/web-scraping/job.xlsx
@@ -397,13 +397,738 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>job_title</v>
+      </c>
+      <c r="B1" t="str">
+        <v>company_name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>location</v>
+      </c>
+      <c r="D1" t="str">
+        <v>job_type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>posted_date</v>
+      </c>
+      <c r="F1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2" xml:space="preserve">
+      <c r="A2" t="str">
+        <v xml:space="preserve">Urgent Requirement for Banking DATA ENTRY Project || No Fees || Salary 35000 to 45000 || Work from Home Job </v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v xml:space="preserve">URGENT HIRING FOR AIRPORT || JOB IN NURSING ANM GNM ANY OTHER QUALIFICATIONS || JOB LOCATION BANGALORE AIRPORT </v>
+      </c>
+      <c r="B3" t="str">
+        <v/>
+      </c>
+      <c r="C3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Nurse - 
+                            Hospital,  Clinic,  Private-House,  Ambulance
+                            + 4 more
+        </v>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
+        <v xml:space="preserve">Part Time Jobs Work From Home Jobs Just Write In your Handwriting or Cursive Handwriting  and Earn From Home </v>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Content Writer - 
+                            Entertainment,  Medical,  Banking-&amp;-Financial-Services,  Technology
+                            + 4 more
+        </v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" xml:space="preserve">
+      <c r="A5" t="str">
+        <v xml:space="preserve">AURANGABAD INTERNATIONAL AIRPORT HRING SECURITY GUARD AND TICKET COUNTER JOBS CURRENT APPLE CANDIDATE IN AIRPORT JOBS VACANCY. </v>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Security/Guard - 
+                            Private-Security,  Armed-Forces
+        </v>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6" t="str">
+        <v xml:space="preserve">Urgent Hiring Driver job for Kempegowda International Airport Bangalore. </v>
+      </c>
+      <c r="B6" t="str">
+        <v/>
+      </c>
+      <c r="C6" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Driver - 
+                            Company-driver,  Private-Driver,  Commercial-Transport-Driver,  Interstate-Driver
+                            + 10 more
+        </v>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7" t="str">
+        <v xml:space="preserve">VACANCY IN AMAZON INDIA FOR HOME-BASED DATA ENTRY JOB  | ALL OVER INDIA VACANCY </v>
+      </c>
+      <c r="B7" t="str">
+        <v/>
+      </c>
+      <c r="C7" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8" t="str">
+        <v xml:space="preserve">URGENT RECRUITMENT IN MUTHOOT FINANCE FOR DATA ENTRY JOB | HOME-BASED </v>
+      </c>
+      <c r="B8" t="str">
+        <v/>
+      </c>
+      <c r="C8" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9" xml:space="preserve">
+      <c r="A9" t="str">
+        <v xml:space="preserve">EARN 30K WORK FROM HOME JOBS DATA ENTRY BACK OFFICE </v>
+      </c>
+      <c r="B9" t="str">
+        <v/>
+      </c>
+      <c r="C9" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10" t="str">
+        <v xml:space="preserve">we have a good jobs in BPO telecaller full time jobs and part time jobs vacancy available </v>
+      </c>
+      <c r="B10" t="str">
+        <v/>
+      </c>
+      <c r="C10" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            BPO/ Telecaller - 
+                            Domestic,  Incoming,  Non Voice,  Outgoing
+                            + 2 more
+        </v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11" xml:space="preserve">
+      <c r="A11" t="str">
+        <v xml:space="preserve">Data Entry jobs in Bangalore </v>
+      </c>
+      <c r="B11" t="str">
+        <v/>
+      </c>
+      <c r="C11" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12" xml:space="preserve">
+      <c r="A12" t="str">
+        <v xml:space="preserve">WORK FROM HOME &amp; PART TIME JOBS CANDIDATES REQUIRED URGENTLY DAILY EARN 30000 WEEKLY PAYMENT, YOU CAN WORK ANYTIME THERE IS NO TIME </v>
+      </c>
+      <c r="B12" t="str">
+        <v/>
+      </c>
+      <c r="C12" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" xml:space="preserve">
+      <c r="A13" t="str">
+        <v xml:space="preserve">Now Requirements Boys Candidates For Therapist Job Vacancy At Artimam Spa Center </v>
+      </c>
+      <c r="B13" t="str">
+        <v/>
+      </c>
+      <c r="C13" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Others
+        </v>
+      </c>
+      <c r="D13" t="str">
+        <v/>
+      </c>
+      <c r="E13" t="str">
+        <v/>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" xml:space="preserve">
+      <c r="A14" t="str">
+        <v xml:space="preserve">Female Massage therapist job - part time </v>
+      </c>
+      <c r="B14" t="str">
+        <v/>
+      </c>
+      <c r="C14" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Beautician - 
+                            Massage
+        </v>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15" xml:space="preserve">
+      <c r="A15" t="str">
+        <v xml:space="preserve">MEESHO part time HOME BASED data entry jobs					 </v>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16" xml:space="preserve">
+      <c r="A16" t="str">
+        <v xml:space="preserve">Simple Data Entry &amp; Form Filling Work home based Job </v>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" xml:space="preserve">
+      <c r="A20" t="str">
+        <v xml:space="preserve">Tata Motors Ltd Mechanical Engineer and all the engineers only freshers candidates can be allowed to apply the job directly joining Freshers Ready --- </v>
+      </c>
+      <c r="B20" t="str">
+        <v/>
+      </c>
+      <c r="C20" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Engineer
+        </v>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <v/>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" xml:space="preserve">
+      <c r="A21" t="str">
+        <v xml:space="preserve">Tata Motors Ltd Mechanical Engineer and all the engineers only freshers candidates can be allowed to apply the job directly joining Freshers Ready --&amp; </v>
+      </c>
+      <c r="B21" t="str">
+        <v/>
+      </c>
+      <c r="C21" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Engineer
+        </v>
+      </c>
+      <c r="D21" t="str">
+        <v/>
+      </c>
+      <c r="E21" t="str">
+        <v/>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" xml:space="preserve">
+      <c r="A22" t="str">
+        <v xml:space="preserve">Tata Motors Ltd Mechanical Engineer and all the engineers only freshers candidates can be allowed to apply the job directly joining Freshers Ready --| </v>
+      </c>
+      <c r="B22" t="str">
+        <v/>
+      </c>
+      <c r="C22" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Engineer
+        </v>
+      </c>
+      <c r="D22" t="str">
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <v/>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23" xml:space="preserve">
+      <c r="A23" t="str">
+        <v xml:space="preserve">Work from Home Job opportunity for MD Dermatologist in India </v>
+      </c>
+      <c r="B23" t="str">
+        <v/>
+      </c>
+      <c r="C23" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Doctor - 
+                            Dermatologist
+        </v>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" xml:space="preserve">
+      <c r="A24" t="str">
+        <v xml:space="preserve">Jobs and Employment </v>
+      </c>
+      <c r="B24" t="str">
+        <v/>
+      </c>
+      <c r="C24" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Business Analyst
+        </v>
+      </c>
+      <c r="D24" t="str">
+        <v/>
+      </c>
+      <c r="E24" t="str">
+        <v/>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25" xml:space="preserve">
+      <c r="A25" t="str">
+        <v xml:space="preserve">Job in Bangalore for freshers  </v>
+      </c>
+      <c r="B25" t="str">
+        <v/>
+      </c>
+      <c r="C25" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Operator/Machinist - 
+                            Laundry
+        </v>
+      </c>
+      <c r="D25" t="str">
+        <v/>
+      </c>
+      <c r="E25" t="str">
+        <v/>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26" xml:space="preserve">
+      <c r="A26" t="str">
+        <v xml:space="preserve">Helper Job in Transport Bhadrak </v>
+      </c>
+      <c r="B26" t="str">
+        <v/>
+      </c>
+      <c r="C26" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Office Assistant/Helper
+        </v>
+      </c>
+      <c r="D26" t="str">
+        <v/>
+      </c>
+      <c r="E26" t="str">
+        <v/>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27" xml:space="preserve">
+      <c r="A27" t="str">
+        <v xml:space="preserve">Book Editing Job </v>
+      </c>
+      <c r="B27" t="str">
+        <v/>
+      </c>
+      <c r="C27" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Data Entry /Back Office
+        </v>
+      </c>
+      <c r="D27" t="str">
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <v/>
+      </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="28" xml:space="preserve">
+      <c r="A28" t="str">
+        <v xml:space="preserve">Auto Driving Job  </v>
+      </c>
+      <c r="B28" t="str">
+        <v/>
+      </c>
+      <c r="C28" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Driver - 
+                            Company-driver,  Commercial-Transport-Driver,  Auto-Driver,  Taxi/Cab
+        </v>
+      </c>
+      <c r="D28" t="str">
+        <v/>
+      </c>
+      <c r="E28" t="str">
+        <v/>
+      </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29" xml:space="preserve">
+      <c r="A29" t="str">
+        <v xml:space="preserve">Ice-cream parlor jobs </v>
+      </c>
+      <c r="B29" t="str">
+        <v/>
+      </c>
+      <c r="C29" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+            Sales - 
+                            Food-and-Beverage-Sales
+        </v>
+      </c>
+      <c r="D29" t="str">
+        <v/>
+      </c>
+      <c r="E29" t="str">
+        <v/>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v/>
+      </c>
+      <c r="B30" t="str">
+        <v/>
+      </c>
+      <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <v/>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <v/>
+      </c>
+      <c r="E31" t="str">
+        <v/>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v/>
+      </c>
+      <c r="B32" t="str">
+        <v/>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <v/>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <v/>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>